<commit_message>
RData qui passe ? plot + clean
</commit_message>
<xml_diff>
--- a/Data/trait_SHOC-HUMAIN.xlsx
+++ b/Data/trait_SHOC-HUMAIN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://lpo061-my.sharepoint.com/personal/suzanne_bonamour_lpo_fr/Documents/2) Data/8) SHOC-humain/SHOC-humain/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="256" documentId="8_{0923755A-BA8D-4E4F-AAD7-767E55E85093}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2AC762C5-5A3D-4054-8C47-B3DF864782D9}"/>
+  <xr:revisionPtr revIDLastSave="270" documentId="8_{0923755A-BA8D-4E4F-AAD7-767E55E85093}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{395D31D6-CD15-4F6B-A49F-B105E3348BA5}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="48">
   <si>
     <t>espece</t>
   </si>
@@ -174,13 +174,16 @@
   </si>
   <si>
     <t>migrateur_simplifie</t>
+  </si>
+  <si>
+    <t>fauneFrance</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -227,6 +230,12 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -248,7 +257,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -260,6 +269,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -598,11 +608,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I34"/>
+  <dimension ref="A1:J34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="K18" sqref="K18"/>
+      <selection pane="topRight" activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -615,7 +625,7 @@
     <col min="6" max="6" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -643,22 +653,25 @@
       <c r="I1" s="10" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J1" s="11" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="D2" s="9" t="s">
         <v>40</v>
       </c>
       <c r="E2" s="6">
-        <v>1250000</v>
+        <v>1500000</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>42</v>
@@ -672,10 +685,13 @@
       <c r="I2" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J2">
+        <v>38967</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
@@ -684,74 +700,80 @@
         <v>9</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="E3" s="6">
-        <v>1500000</v>
+        <v>1650000</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>42</v>
       </c>
       <c r="G3" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="H3" t="s">
         <v>3</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+      <c r="J3">
+        <v>17030</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="D4" s="9" t="s">
         <v>40</v>
       </c>
       <c r="E4" s="6">
-        <v>3250000</v>
+        <v>45000</v>
       </c>
       <c r="F4" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G4" t="s">
+        <v>3</v>
+      </c>
+      <c r="H4" t="s">
+        <v>3</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="J4">
+        <v>13561</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="E5" s="6">
+        <v>300000</v>
+      </c>
+      <c r="F5" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="G4" t="s">
-        <v>3</v>
-      </c>
-      <c r="H4" t="s">
-        <v>9</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" t="s">
-        <v>3</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="E5" s="6">
-        <v>45000</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>43</v>
-      </c>
       <c r="G5" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="H5" t="s">
         <v>3</v>
@@ -759,25 +781,28 @@
       <c r="I5" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J5">
+        <v>10266</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" t="s">
-        <v>3</v>
+        <v>19</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="D6" s="9" t="s">
         <v>44</v>
       </c>
       <c r="E6" s="6">
-        <v>300000</v>
+        <v>1500000</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G6" t="s">
         <v>9</v>
@@ -786,14 +811,17 @@
         <v>3</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+      <c r="J6">
+        <v>55160</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>25</v>
-      </c>
-      <c r="B7" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" t="s">
         <v>5</v>
       </c>
       <c r="C7" t="s">
@@ -803,39 +831,42 @@
         <v>45</v>
       </c>
       <c r="E7" s="6">
-        <v>400000</v>
+        <v>225000</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>3</v>
+        <v>43</v>
+      </c>
+      <c r="G7" t="s">
+        <v>9</v>
       </c>
       <c r="H7" t="s">
         <v>3</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+      <c r="J7">
+        <v>28283</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="B8" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="D8" s="9" t="s">
         <v>45</v>
       </c>
       <c r="E8" s="6">
-        <v>800000</v>
+        <v>2750000</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G8" t="s">
         <v>9</v>
@@ -844,111 +875,123 @@
         <v>3</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+      <c r="J8">
+        <v>79503</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B9" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C9" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="E9" s="6">
-        <v>75000</v>
+        <v>700000</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G9" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="H9" t="s">
         <v>3</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+      <c r="J9">
+        <v>50338</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>32</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>5</v>
+        <v>7</v>
+      </c>
+      <c r="B10" t="s">
+        <v>3</v>
       </c>
       <c r="C10" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="D10" s="9" t="s">
         <v>40</v>
       </c>
       <c r="E10" s="6">
-        <v>650000</v>
+        <v>1250000</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>42</v>
       </c>
       <c r="G10" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="H10" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="I10" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J10">
+        <v>31606</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" t="s">
         <v>9</v>
       </c>
       <c r="D11" s="9" t="s">
         <v>45</v>
       </c>
       <c r="E11" s="6">
-        <v>22500</v>
+        <v>400000</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="G11" t="s">
-        <v>9</v>
+        <v>42</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>3</v>
       </c>
       <c r="H11" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="I11" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J11">
+        <v>24458</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>11</v>
-      </c>
-      <c r="B12" t="s">
-        <v>9</v>
-      </c>
-      <c r="C12" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>9</v>
       </c>
       <c r="D12" s="9" t="s">
         <v>45</v>
       </c>
       <c r="E12" s="6">
-        <v>750000</v>
+        <v>22500</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>43</v>
@@ -962,13 +1005,16 @@
       <c r="I12" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J12">
+        <v>10888</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>30</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>5</v>
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>9</v>
       </c>
       <c r="C13" t="s">
         <v>9</v>
@@ -991,86 +1037,95 @@
       <c r="I13" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J13">
+        <v>15848</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C14" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E14" s="6">
-        <v>225000</v>
+        <v>80000</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="G14" t="s">
-        <v>3</v>
+      <c r="G14" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="H14" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="I14" s="4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J14">
+        <v>22515</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>13</v>
-      </c>
-      <c r="B15" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C15" t="s">
         <v>9</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E15" s="6">
-        <v>80000</v>
+        <v>6500000</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>9</v>
+        <v>43</v>
+      </c>
+      <c r="G15" t="s">
+        <v>3</v>
       </c>
       <c r="H15" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="I15" s="4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J15">
+        <v>153806</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>26</v>
-      </c>
-      <c r="B16" t="s">
-        <v>3</v>
+        <v>21</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="C16" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="D16" s="9" t="s">
         <v>45</v>
       </c>
       <c r="E16" s="6">
-        <v>700000</v>
+        <v>3250000</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>43</v>
       </c>
       <c r="G16" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="H16" t="s">
         <v>3</v>
@@ -1078,10 +1133,13 @@
       <c r="I16" s="4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J16">
+        <v>146459</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>5</v>
@@ -1093,24 +1151,27 @@
         <v>45</v>
       </c>
       <c r="E17" s="6">
-        <v>6500000</v>
+        <v>750000</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>43</v>
       </c>
       <c r="G17" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="H17" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="I17" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="J17">
+        <v>10999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="B18" t="s">
         <v>3</v>
@@ -1122,65 +1183,71 @@
         <v>45</v>
       </c>
       <c r="E18" s="6">
+        <v>800000</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G18" t="s">
+        <v>9</v>
+      </c>
+      <c r="H18" t="s">
+        <v>3</v>
+      </c>
+      <c r="I18" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="J18">
+        <v>25777</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19" t="s">
+        <v>3</v>
+      </c>
+      <c r="C19" t="s">
+        <v>3</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="E19" s="6">
+        <v>225000</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G19" t="s">
+        <v>3</v>
+      </c>
+      <c r="H19" t="s">
+        <v>3</v>
+      </c>
+      <c r="I19" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="J19">
+        <v>34554</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>14</v>
+      </c>
+      <c r="B20" t="s">
+        <v>3</v>
+      </c>
+      <c r="C20" t="s">
+        <v>3</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="E20" s="6">
         <v>525000</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="G18" t="s">
-        <v>3</v>
-      </c>
-      <c r="H18" t="s">
-        <v>3</v>
-      </c>
-      <c r="I18" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C19" t="s">
-        <v>9</v>
-      </c>
-      <c r="D19" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="E19" s="6">
-        <v>4500000</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="G19" t="s">
-        <v>3</v>
-      </c>
-      <c r="H19" t="s">
-        <v>3</v>
-      </c>
-      <c r="I19" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>18</v>
-      </c>
-      <c r="B20" t="s">
-        <v>3</v>
-      </c>
-      <c r="C20" t="s">
-        <v>3</v>
-      </c>
-      <c r="D20" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="E20" s="6">
-        <v>1300000</v>
       </c>
       <c r="F20" s="2" t="s">
         <v>43</v>
@@ -1194,28 +1261,31 @@
       <c r="I20" s="4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J20">
+        <v>111545</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>29</v>
-      </c>
-      <c r="B21" t="s">
-        <v>3</v>
+        <v>8</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="C21" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="E21" s="6">
-        <v>4000000</v>
+        <v>2500000</v>
       </c>
       <c r="F21" s="2" t="s">
         <v>43</v>
       </c>
       <c r="G21" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="H21" t="s">
         <v>3</v>
@@ -1223,12 +1293,15 @@
       <c r="I21" s="4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J21">
+        <v>109882</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>17</v>
-      </c>
-      <c r="B22" t="s">
+        <v>20</v>
+      </c>
+      <c r="B22" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C22" t="s">
@@ -1238,10 +1311,10 @@
         <v>44</v>
       </c>
       <c r="E22" s="6">
-        <v>1650000</v>
+        <v>9000000</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G22" t="s">
         <v>9</v>
@@ -1252,10 +1325,13 @@
       <c r="I22" s="4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J22">
+        <v>165703</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="B23" t="s">
         <v>9</v>
@@ -1264,10 +1340,10 @@
         <v>9</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="E23" s="6">
-        <v>1500</v>
+        <v>75000</v>
       </c>
       <c r="F23" s="2" t="s">
         <v>42</v>
@@ -1276,42 +1352,48 @@
         <v>9</v>
       </c>
       <c r="H23" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="I23" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="J23">
+        <v>26940</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>33</v>
-      </c>
-      <c r="B24" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B24" t="s">
         <v>5</v>
       </c>
       <c r="C24" t="s">
         <v>9</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="E24" s="6">
-        <v>1500000</v>
+        <v>3250000</v>
       </c>
       <c r="F24" s="2" t="s">
         <v>42</v>
       </c>
       <c r="G24" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="H24" t="s">
         <v>9</v>
       </c>
       <c r="I24" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="J24">
+        <v>29181</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>34</v>
       </c>
@@ -1339,10 +1421,13 @@
       <c r="I25" s="4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J25">
+        <v>17069</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>5</v>
@@ -1351,45 +1436,48 @@
         <v>9</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="E26" s="6">
-        <v>1500000</v>
+        <v>650000</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G26" t="s">
         <v>9</v>
       </c>
       <c r="H26" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="I26" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>4</v>
-      </c>
-      <c r="B27" t="s">
+        <v>3</v>
+      </c>
+      <c r="J26">
+        <v>12357</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B27" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C27" t="s">
         <v>9</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="E27" s="6">
-        <v>225000</v>
+        <v>4500000</v>
       </c>
       <c r="F27" s="2" t="s">
         <v>43</v>
       </c>
       <c r="G27" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="H27" t="s">
         <v>3</v>
@@ -1397,57 +1485,63 @@
       <c r="I27" s="4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J27">
+        <v>175406</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B28" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C28" t="s">
         <v>9</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E28" s="6">
-        <v>2750000</v>
+        <v>1500</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G28" t="s">
         <v>9</v>
       </c>
       <c r="H28" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="I28" s="4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J28">
+        <v>24903</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>21</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>5</v>
+        <v>18</v>
+      </c>
+      <c r="B29" t="s">
+        <v>3</v>
       </c>
       <c r="C29" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E29" s="6">
-        <v>3250000</v>
+        <v>1300000</v>
       </c>
       <c r="F29" s="2" t="s">
         <v>43</v>
       </c>
       <c r="G29" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="H29" t="s">
         <v>3</v>
@@ -1455,28 +1549,31 @@
       <c r="I29" s="4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J29">
+        <v>65618</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>8</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>5</v>
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>3</v>
       </c>
       <c r="C30" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="E30" s="6">
-        <v>2500000</v>
+        <v>4000000</v>
       </c>
       <c r="F30" s="2" t="s">
         <v>43</v>
       </c>
       <c r="G30" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="H30" t="s">
         <v>3</v>
@@ -1484,10 +1581,13 @@
       <c r="I30" s="4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J30">
+        <v>50172</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>5</v>
@@ -1499,22 +1599,25 @@
         <v>44</v>
       </c>
       <c r="E31" s="6">
-        <v>9000000</v>
+        <v>1500000</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G31" t="s">
         <v>9</v>
       </c>
       <c r="H31" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="I31" s="4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J31">
+        <v>34169</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
     </row>
@@ -1525,8 +1628,8 @@
       <c r="F34" s="3"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I32">
-    <sortCondition ref="I1:I32"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I34">
+    <sortCondition ref="A1:A34"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>